<commit_message>
add list view for teams
</commit_message>
<xml_diff>
--- a/src/assets/Transactions_Import_Template.xlsx
+++ b/src/assets/Transactions_Import_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Groflex\Repositories\Old groflex repos\groflex-india-app-react\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B257B01-9B09-47D7-A80D-46569536B6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E911F510-648F-4808-A559-219C8298C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Groflex Transactions Import</t>
   </si>
@@ -151,6 +151,28 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Amount</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Please match the 'Account name' column in the groflex transactions list with the 'Description' column of this excel file</t>
     </r>
   </si>
 </sst>
@@ -158,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +224,20 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -283,16 +319,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,16 +619,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.77734375" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="31.21875" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" customWidth="1"/>
@@ -591,48 +636,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changes merge for other modules and side bar
</commit_message>
<xml_diff>
--- a/src/assets/Transactions_Import_Template.xlsx
+++ b/src/assets/Transactions_Import_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Groflex\Repositories\Old groflex repos\groflex-india-app-react\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B257B01-9B09-47D7-A80D-46569536B6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E911F510-648F-4808-A559-219C8298C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Groflex Transactions Import</t>
   </si>
@@ -151,6 +151,28 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Amount</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Please match the 'Account name' column in the groflex transactions list with the 'Description' column of this excel file</t>
     </r>
   </si>
 </sst>
@@ -158,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +224,20 @@
       <name val="Segoe UI"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -283,16 +319,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,16 +619,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.77734375" customWidth="1"/>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="31.21875" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" customWidth="1"/>
@@ -591,48 +636,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" ht="24.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="A2:I2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>